<commit_message>
lesson 3. database desing, fix the tables
</commit_message>
<xml_diff>
--- a/Geekbrains.ru/Database design.xlsx
+++ b/Geekbrains.ru/Database design.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="Плохо спроектированная БД" sheetId="3" r:id="rId1"/>
-    <sheet name="Нарушена 1-я НФ" sheetId="2" r:id="rId2"/>
-    <sheet name="Уже лучше. Но нарешуна 1 НФ" sheetId="4" r:id="rId3"/>
+    <sheet name="Плохой проект БД" sheetId="3" r:id="rId1"/>
+    <sheet name="Нарушена 1 НФ" sheetId="2" r:id="rId2"/>
+    <sheet name="Уже лучше. Но нарушена 1 НФ" sheetId="4" r:id="rId3"/>
     <sheet name="1 НФ" sheetId="5" r:id="rId4"/>
     <sheet name="Нарушена 2 НФ" sheetId="6" r:id="rId5"/>
     <sheet name="2НФ" sheetId="7" r:id="rId6"/>
     <sheet name="3НФ" sheetId="8" r:id="rId7"/>
     <sheet name="Товары" sheetId="1" state="hidden" r:id="rId8"/>
+    <sheet name="Лист1" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'2НФ'!$A$2:$D$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Нарушена 1-я НФ'!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Уже лучше. Но нарешуна 1 НФ'!$A$1:$C$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Нарушена 1 НФ'!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Уже лучше. Но нарушена 1 НФ'!$A$1:$C$5</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -30,8 +31,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Автор</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Автор:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+первичный ключ</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="36">
   <si>
     <t>Marc  O'Polo</t>
   </si>
@@ -145,7 +180,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +196,19 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -275,6 +323,24 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -286,24 +352,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,7 +659,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -811,7 +859,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="L19" sqref="L19:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -894,6 +942,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -902,7 +951,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1009,7 +1058,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1022,12 +1071,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
@@ -1100,11 +1149,11 @@
       </c>
     </row>
     <row r="10" spans="1:4" s="10" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="6" t="s">
@@ -1150,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1167,16 +1216,16 @@
     <col min="7" max="7" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" customHeight="1">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:6" ht="24.95" customHeight="1">
+      <c r="A1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1">
+    <row r="2" spans="1:6" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1192,149 +1241,87 @@
       <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="18">
+        <v>1</v>
+      </c>
+      <c r="C3" s="18">
+        <v>1</v>
+      </c>
+      <c r="D3" s="18">
+        <v>1</v>
+      </c>
+      <c r="E3" s="18">
+        <v>15980</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="18">
+        <v>2</v>
+      </c>
+      <c r="C4" s="18">
+        <v>2</v>
+      </c>
+      <c r="D4" s="18">
+        <v>1</v>
+      </c>
+      <c r="E4" s="18">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="18">
         <v>3</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="22">
-        <v>1</v>
-      </c>
-      <c r="C3" s="22">
-        <v>1</v>
-      </c>
-      <c r="D3" s="22">
-        <v>1</v>
-      </c>
-      <c r="E3" s="22">
-        <v>15980</v>
-      </c>
-      <c r="F3" s="23">
-        <v>1</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="24">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="22">
-        <v>2</v>
-      </c>
-      <c r="C4" s="22">
-        <v>2</v>
-      </c>
-      <c r="D4" s="22">
-        <v>1</v>
-      </c>
-      <c r="E4" s="22">
-        <v>1090</v>
-      </c>
-      <c r="F4" s="23">
-        <v>1</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="24">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="22">
-        <v>3</v>
-      </c>
-      <c r="C5" s="22">
-        <v>1</v>
-      </c>
-      <c r="D5" s="22">
-        <v>1</v>
-      </c>
-      <c r="E5" s="22">
+      <c r="C5" s="18">
+        <v>1</v>
+      </c>
+      <c r="D5" s="18">
+        <v>1</v>
+      </c>
+      <c r="E5" s="18">
         <v>13990</v>
       </c>
-      <c r="F5" s="23">
-        <v>1</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="24">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="22" t="s">
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="22">
-        <v>2</v>
-      </c>
-      <c r="C6" s="22">
-        <v>2</v>
-      </c>
-      <c r="D6" s="22">
-        <v>2</v>
-      </c>
-      <c r="E6" s="22">
+      <c r="B6" s="18">
+        <v>2</v>
+      </c>
+      <c r="C6" s="18">
+        <v>2</v>
+      </c>
+      <c r="D6" s="18">
+        <v>2</v>
+      </c>
+      <c r="E6" s="18">
         <v>1490</v>
       </c>
-      <c r="F6" s="23">
-        <v>2</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4">
-        <v>2</v>
-      </c>
-      <c r="C7" s="4">
-        <v>2</v>
-      </c>
-      <c r="D7" s="4">
-        <v>8</v>
-      </c>
-      <c r="E7" s="4">
-        <v>16789</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A10" s="16" t="s">
+    </row>
+    <row r="10" spans="1:6" s="10" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="E10" s="18" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="E10" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="18"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="F10" s="24"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="6" t="s">
         <v>25</v>
       </c>
@@ -1351,7 +1338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:6">
       <c r="A12" s="7">
         <v>1</v>
       </c>
@@ -1368,7 +1355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:6">
       <c r="A13" s="7">
         <v>2</v>
       </c>
@@ -1385,16 +1372,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="19">
-        <v>3</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="21">
-        <v>0.15</v>
-      </c>
+    <row r="14" spans="1:6">
+      <c r="A14" s="15"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
       <c r="E14" s="14">
         <v>3</v>
       </c>
@@ -1402,11 +1383,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="10" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A17" s="17" t="s">
+    <row r="17" spans="1:2" s="10" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A17" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="17"/>
+      <c r="B17" s="23"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="11" t="s">
@@ -1440,6 +1421,7 @@
     <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1548,4 +1530,299 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="28.5" customHeight="1">
+      <c r="A1" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="18">
+        <v>1</v>
+      </c>
+      <c r="C3" s="18">
+        <v>1</v>
+      </c>
+      <c r="D3" s="18">
+        <v>1</v>
+      </c>
+      <c r="E3" s="18">
+        <v>15980</v>
+      </c>
+      <c r="F3" s="19">
+        <v>1</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="20">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="18">
+        <v>2</v>
+      </c>
+      <c r="C4" s="18">
+        <v>2</v>
+      </c>
+      <c r="D4" s="18">
+        <v>1</v>
+      </c>
+      <c r="E4" s="18">
+        <v>1090</v>
+      </c>
+      <c r="F4" s="19">
+        <v>1</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="20">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="18">
+        <v>3</v>
+      </c>
+      <c r="C5" s="18">
+        <v>1</v>
+      </c>
+      <c r="D5" s="18">
+        <v>1</v>
+      </c>
+      <c r="E5" s="18">
+        <v>13990</v>
+      </c>
+      <c r="F5" s="19">
+        <v>1</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="20">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="18">
+        <v>2</v>
+      </c>
+      <c r="C6" s="18">
+        <v>2</v>
+      </c>
+      <c r="D6" s="18">
+        <v>2</v>
+      </c>
+      <c r="E6" s="18">
+        <v>1490</v>
+      </c>
+      <c r="F6" s="19">
+        <v>2</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4">
+        <v>16789</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="10" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A10" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="E10" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="24"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="7">
+        <v>1</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="E12" s="14">
+        <v>1</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="7">
+        <v>2</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="14">
+        <v>2</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="15">
+        <v>3</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="17">
+        <v>0.15</v>
+      </c>
+      <c r="E14" s="14">
+        <v>3</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="10" customFormat="1" ht="27.75" customHeight="1">
+      <c r="A17" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="23"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="12">
+        <v>1</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="12">
+        <v>2</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A17:B17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>